<commit_message>
Removed FIPS Country Code and Added nc:LocationStateName
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Court_Case_Filing/artifacts/service_model/information_model/IEPD/documentation/impl-artifacts/vermont/Citation_Case_Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Court_Case_Filing/artifacts/service_model/information_model/IEPD/documentation/impl-artifacts/vermont/Citation_Case_Mapping.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-28455" yWindow="5925" windowWidth="29040" windowHeight="15885"/>
+    <workbookView xWindow="6200" yWindow="2120" windowWidth="29040" windowHeight="15500"/>
   </bookViews>
   <sheets>
     <sheet name="eCitation" sheetId="1" r:id="rId1"/>
@@ -695,9 +695,6 @@
     <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationCityName</t>
   </si>
   <si>
-    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationCountryFIPS10-4Code</t>
-  </si>
-  <si>
     <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationPostalCode</t>
   </si>
   <si>
@@ -863,9 +860,6 @@
     <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/ecf:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationCityName</t>
   </si>
   <si>
-    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/ecf:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationCountryFIPS10-4Code</t>
-  </si>
-  <si>
     <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/ecf:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationPostalCode</t>
   </si>
   <si>
@@ -885,6 +879,12 @@
   </si>
   <si>
     <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/j:CitationAgency/nc:OrganizationPrimaryContactInformation/nc:ContactEntity/ecf:EntityOrganization/nc:OrganizationIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationStateName</t>
+  </si>
+  <si>
+    <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/ecf:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationStateName</t>
   </si>
 </sst>
 </file>
@@ -892,7 +892,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -1849,7 +1849,7 @@
     <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2915,22 +2915,22 @@
   <dimension ref="A1:E87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B67" sqref="B67"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="37.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="39.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="39.5" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="100.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="48.140625" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="2"/>
+    <col min="4" max="4" width="21.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="100.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="48.1640625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="9" customFormat="1" ht="28">
       <c r="A1" s="1" t="s">
         <v>202</v>
       </c>
@@ -2947,7 +2947,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="19" customHeight="1">
       <c r="A2" s="11" t="s">
         <v>81</v>
       </c>
@@ -2956,7 +2956,7 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="28">
       <c r="A3" s="14" t="s">
         <v>189</v>
       </c>
@@ -2973,7 +2973,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="3" customFormat="1">
       <c r="A4" s="3" t="s">
         <v>190</v>
       </c>
@@ -2990,7 +2990,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A5" s="6" t="s">
         <v>47</v>
       </c>
@@ -3007,7 +3007,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A6" s="6" t="s">
         <v>191</v>
       </c>
@@ -3024,7 +3024,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A7" s="6" t="s">
         <v>192</v>
       </c>
@@ -3041,7 +3041,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="10" t="s">
         <v>62</v>
       </c>
@@ -3050,7 +3050,7 @@
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="28">
       <c r="A9" s="15" t="s">
         <v>3</v>
       </c>
@@ -3064,7 +3064,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="10" t="s">
         <v>198</v>
       </c>
@@ -3073,7 +3073,7 @@
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="42">
       <c r="A11" s="12" t="s">
         <v>3</v>
       </c>
@@ -3087,7 +3087,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="10" t="s">
         <v>63</v>
       </c>
@@ -3096,7 +3096,7 @@
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="42">
       <c r="A13" s="14" t="s">
         <v>64</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="42">
       <c r="A14" s="14" t="s">
         <v>2</v>
       </c>
@@ -3130,7 +3130,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="42">
       <c r="A15" s="14" t="s">
         <v>94</v>
       </c>
@@ -3147,7 +3147,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="70">
       <c r="A16" s="14" t="s">
         <v>57</v>
       </c>
@@ -3164,7 +3164,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="56">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
@@ -3181,7 +3181,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="56">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
@@ -3195,10 +3195,10 @@
         <v>120</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="3" customFormat="1" ht="56">
       <c r="A19" s="3" t="s">
         <v>6</v>
       </c>
@@ -3212,10 +3212,10 @@
         <v>127</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="56">
       <c r="A20" s="14" t="s">
         <v>1</v>
       </c>
@@ -3229,10 +3229,10 @@
         <v>41444812</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="56">
       <c r="A21" s="14" t="s">
         <v>90</v>
       </c>
@@ -3246,10 +3246,10 @@
         <v>120</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="56">
       <c r="A22" s="12" t="s">
         <v>88</v>
       </c>
@@ -3263,10 +3263,10 @@
         <v>12345678</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="3" customFormat="1" ht="98">
       <c r="A23" s="3" t="s">
         <v>15</v>
       </c>
@@ -3280,10 +3280,10 @@
         <v>8023631111</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="3" customFormat="1" ht="98">
       <c r="A24" s="3" t="s">
         <v>16</v>
       </c>
@@ -3297,10 +3297,10 @@
         <v>8023631112</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A25" s="3" t="s">
         <v>17</v>
       </c>
@@ -3314,10 +3314,10 @@
         <v>24014</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A26" s="3" t="s">
         <v>65</v>
       </c>
@@ -3331,10 +3331,10 @@
         <v>128</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="3" customFormat="1" ht="56">
       <c r="A27" s="16" t="s">
         <v>155</v>
       </c>
@@ -3348,10 +3348,10 @@
         <v>129</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A28" s="3" t="s">
         <v>19</v>
       </c>
@@ -3365,10 +3365,10 @@
         <v>130</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A29" s="3" t="s">
         <v>156</v>
       </c>
@@ -3376,10 +3376,10 @@
         <v>164</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A30" s="3" t="s">
         <v>20</v>
       </c>
@@ -3393,10 +3393,10 @@
         <v>135</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A31" s="3" t="s">
         <v>116</v>
       </c>
@@ -3404,10 +3404,10 @@
         <v>165</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A32" s="3" t="s">
         <v>153</v>
       </c>
@@ -3421,10 +3421,10 @@
         <v>131</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A33" s="3" t="s">
         <v>154</v>
       </c>
@@ -3438,10 +3438,10 @@
         <v>131</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" s="10" t="s">
         <v>84</v>
       </c>
@@ -3450,7 +3450,7 @@
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
     </row>
-    <row r="35" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A35" s="3" t="s">
         <v>66</v>
       </c>
@@ -3464,10 +3464,10 @@
         <v>161</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="3" customFormat="1" ht="56">
       <c r="A36" s="3" t="s">
         <v>95</v>
       </c>
@@ -3478,10 +3478,10 @@
         <v>132</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="3" customFormat="1" ht="56">
       <c r="A37" s="3" t="s">
         <v>96</v>
       </c>
@@ -3495,10 +3495,10 @@
         <v>120</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A38" s="3" t="s">
         <v>97</v>
       </c>
@@ -3512,10 +3512,10 @@
         <v>2015</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A39" s="3" t="s">
         <v>98</v>
       </c>
@@ -3529,10 +3529,10 @@
         <v>134</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A40" s="3" t="s">
         <v>99</v>
       </c>
@@ -3546,10 +3546,10 @@
         <v>135</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A41" s="3" t="s">
         <v>100</v>
       </c>
@@ -3563,10 +3563,10 @@
         <v>136</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A42" s="16" t="s">
         <v>152</v>
       </c>
@@ -3580,10 +3580,10 @@
         <v>0</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" s="3" customFormat="1" ht="56">
       <c r="A43" s="6" t="s">
         <v>101</v>
       </c>
@@ -3597,10 +3597,10 @@
         <v>0</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" s="10" t="s">
         <v>82</v>
       </c>
@@ -3609,7 +3609,7 @@
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
     </row>
-    <row r="45" spans="1:5" s="3" customFormat="1" ht="68.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" s="3" customFormat="1" ht="68" customHeight="1">
       <c r="A45" s="14" t="s">
         <v>102</v>
       </c>
@@ -3623,10 +3623,10 @@
         <v>121</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A46" s="3" t="s">
         <v>103</v>
       </c>
@@ -3640,10 +3640,10 @@
         <v>137</v>
       </c>
       <c r="E46" s="15" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" s="3" customFormat="1" ht="56">
       <c r="A47" s="3" t="s">
         <v>104</v>
       </c>
@@ -3654,10 +3654,10 @@
         <v>28</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" s="3" customFormat="1" ht="56">
       <c r="A48" s="13" t="s">
         <v>105</v>
       </c>
@@ -3671,10 +3671,10 @@
         <v>138</v>
       </c>
       <c r="E48" s="15" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" s="3" customFormat="1" ht="56">
       <c r="A49" s="13" t="s">
         <v>106</v>
       </c>
@@ -3688,10 +3688,10 @@
         <v>139</v>
       </c>
       <c r="E49" s="15" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A50" s="3" t="s">
         <v>107</v>
       </c>
@@ -3705,10 +3705,10 @@
         <v>140</v>
       </c>
       <c r="E50" s="15" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A51" s="3" t="s">
         <v>108</v>
       </c>
@@ -3722,10 +3722,10 @@
         <v>0.2</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" s="3" customFormat="1" ht="56">
       <c r="A52" s="3" t="s">
         <v>33</v>
       </c>
@@ -3739,10 +3739,10 @@
         <v>30</v>
       </c>
       <c r="E52" s="15" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" s="3" customFormat="1" ht="56">
       <c r="A53" s="3" t="s">
         <v>162</v>
       </c>
@@ -3753,10 +3753,10 @@
         <v>163</v>
       </c>
       <c r="E53" s="15" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A54" s="3" t="s">
         <v>34</v>
       </c>
@@ -3770,10 +3770,10 @@
         <v>40</v>
       </c>
       <c r="E54" s="15" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" s="3" customFormat="1" ht="56">
       <c r="A55" s="3" t="s">
         <v>162</v>
       </c>
@@ -3784,10 +3784,10 @@
         <v>163</v>
       </c>
       <c r="E55" s="15" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" s="3" customFormat="1" ht="56">
       <c r="A56" s="3" t="s">
         <v>109</v>
       </c>
@@ -3801,10 +3801,10 @@
         <v>0</v>
       </c>
       <c r="E56" s="15" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" s="3" customFormat="1" ht="56">
       <c r="A57" s="6" t="s">
         <v>110</v>
       </c>
@@ -3818,10 +3818,10 @@
         <v>0</v>
       </c>
       <c r="E57" s="15" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" s="3" customFormat="1" ht="56">
       <c r="A58" s="6" t="s">
         <v>111</v>
       </c>
@@ -3835,10 +3835,10 @@
         <v>0</v>
       </c>
       <c r="E58" s="15" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="56">
       <c r="A59" s="12" t="s">
         <v>205</v>
       </c>
@@ -3852,10 +3852,10 @@
         <v>1</v>
       </c>
       <c r="E59" s="15" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="56">
       <c r="A60" s="12" t="s">
         <v>206</v>
       </c>
@@ -3869,10 +3869,10 @@
         <v>1</v>
       </c>
       <c r="E60" s="15" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="56">
       <c r="A61" s="12" t="s">
         <v>207</v>
       </c>
@@ -3886,10 +3886,10 @@
         <v>1</v>
       </c>
       <c r="E61" s="15" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="56">
       <c r="A62" s="12" t="s">
         <v>208</v>
       </c>
@@ -3900,10 +3900,10 @@
         <v>87</v>
       </c>
       <c r="E62" s="15" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
       <c r="A63" s="10" t="s">
         <v>83</v>
       </c>
@@ -3912,7 +3912,7 @@
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
     </row>
-    <row r="64" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A64" s="6" t="s">
         <v>159</v>
       </c>
@@ -3926,10 +3926,10 @@
         <v>142</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A65" s="6" t="s">
         <v>112</v>
       </c>
@@ -3943,10 +3943,10 @@
         <v>141</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A66" s="6" t="s">
         <v>158</v>
       </c>
@@ -3960,10 +3960,10 @@
         <v>143</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A67" s="3" t="s">
         <v>113</v>
       </c>
@@ -3977,10 +3977,10 @@
         <v>144</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A68" s="6" t="s">
         <v>160</v>
       </c>
@@ -3994,10 +3994,10 @@
         <v>0</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A69" s="6" t="s">
         <v>114</v>
       </c>
@@ -4011,10 +4011,10 @@
         <v>2</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A70" s="6" t="s">
         <v>117</v>
       </c>
@@ -4028,10 +4028,10 @@
         <v>47</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A71" s="6" t="s">
         <v>118</v>
       </c>
@@ -4045,10 +4045,10 @@
         <v>1197</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
       <c r="A72" s="10" t="s">
         <v>85</v>
       </c>
@@ -4057,7 +4057,7 @@
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
     </row>
-    <row r="73" spans="1:5" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" s="3" customFormat="1" ht="56">
       <c r="A73" s="3" t="s">
         <v>52</v>
       </c>
@@ -4071,10 +4071,10 @@
         <v>145</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A74" s="3" t="s">
         <v>209</v>
       </c>
@@ -4088,10 +4088,10 @@
         <v>211</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A75" s="3" t="s">
         <v>115</v>
       </c>
@@ -4105,15 +4105,15 @@
         <v>12345</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A76" s="3" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>53</v>
@@ -4122,10 +4122,10 @@
         <v>146</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A77" s="3" t="s">
         <v>54</v>
       </c>
@@ -4139,10 +4139,10 @@
         <v>147</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
       <c r="A78" s="10" t="s">
         <v>86</v>
       </c>
@@ -4151,7 +4151,7 @@
       <c r="D78" s="5"/>
       <c r="E78" s="5"/>
     </row>
-    <row r="79" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" ht="42">
       <c r="A79" s="3" t="s">
         <v>2</v>
       </c>
@@ -4165,10 +4165,10 @@
         <v>148</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="42">
       <c r="A80" s="14" t="s">
         <v>64</v>
       </c>
@@ -4182,10 +4182,10 @@
         <v>122</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="56">
       <c r="A81" s="3" t="s">
         <v>57</v>
       </c>
@@ -4199,10 +4199,10 @@
         <v>149</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="56">
       <c r="A82" s="3" t="s">
         <v>4</v>
       </c>
@@ -4216,10 +4216,10 @@
         <v>150</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="56">
       <c r="A83" s="3" t="s">
         <v>5</v>
       </c>
@@ -4233,10 +4233,10 @@
         <v>120</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="56">
       <c r="A84" s="3" t="s">
         <v>6</v>
       </c>
@@ -4250,10 +4250,10 @@
         <v>151</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
       <c r="A85" s="10" t="s">
         <v>196</v>
       </c>
@@ -4262,7 +4262,7 @@
       <c r="D85" s="5"/>
       <c r="E85" s="5"/>
     </row>
-    <row r="86" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" ht="56">
       <c r="A86" s="12" t="s">
         <v>89</v>
       </c>
@@ -4276,10 +4276,10 @@
         <v>0</v>
       </c>
       <c r="E86" s="15" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" ht="119.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="119" customHeight="1">
       <c r="A87" s="17" t="s">
         <v>204</v>
       </c>

</xml_diff>

<commit_message>
Added CitationIssuedLocation to IEPD.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Court_Case_Filing/artifacts/service_model/information_model/IEPD/documentation/impl-artifacts/vermont/Citation_Case_Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Court_Case_Filing/artifacts/service_model/information_model/IEPD/documentation/impl-artifacts/vermont/Citation_Case_Mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6200" yWindow="2120" windowWidth="29040" windowHeight="15500"/>
+    <workbookView xWindow="1700" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="eCitation" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="291">
   <si>
     <t>Description</t>
   </si>
@@ -885,6 +885,15 @@
   </si>
   <si>
     <t>/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/ecf:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationStateName</t>
+  </si>
+  <si>
+    <t>Citation Issued Loction</t>
+  </si>
+  <si>
+    <t>Location where citation was issued.</t>
+  </si>
+  <si>
+    <t>cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/ojb-cit-ext:CitationAugmentation/ojb-cit-ext:CitationIssuedLocation</t>
   </si>
 </sst>
 </file>
@@ -2912,11 +2921,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E87"/>
+  <dimension ref="A1:E88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D83" sqref="D83"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3041,1255 +3050,1266 @@
         <v>216</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="10" t="s">
+    <row r="8" spans="1:5" s="3" customFormat="1" ht="28">
+      <c r="A8" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="1:5" ht="28">
-      <c r="A9" s="15" t="s">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" ht="28">
+      <c r="A10" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E10" s="15" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="10" t="s">
+    <row r="11" spans="1:5">
+      <c r="A11" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="1:5" ht="42">
-      <c r="A11" s="12" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" ht="42">
+      <c r="A12" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E12" s="15" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="10" t="s">
+    <row r="13" spans="1:5">
+      <c r="A13" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:5" ht="42">
-      <c r="A13" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>219</v>
-      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5" ht="42">
       <c r="A14" s="14" t="s">
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="42">
       <c r="A15" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="42">
+      <c r="A16" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E16" s="15" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="70">
-      <c r="A16" s="14" t="s">
+    <row r="17" spans="1:5" ht="70">
+      <c r="A17" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="E17" s="15" t="s">
         <v>222</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="56">
-      <c r="A17" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="56">
       <c r="A18" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="56">
+      <c r="A19" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="E19" s="15" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="3" customFormat="1" ht="56">
-      <c r="A19" s="3" t="s">
+    <row r="20" spans="1:5" s="3" customFormat="1" ht="56">
+      <c r="A20" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B20" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="E20" s="15" t="s">
         <v>224</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="56">
-      <c r="A20" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="2">
-        <v>41444812</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="56">
       <c r="A21" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="2">
+        <v>41444812</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="56">
+      <c r="A22" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E22" s="15" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="56">
-      <c r="A22" s="12" t="s">
+    <row r="23" spans="1:5" ht="56">
+      <c r="A23" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D23" s="2">
         <v>12345678</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="E23" s="15" t="s">
         <v>227</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" s="3" customFormat="1" ht="98">
-      <c r="A23" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" s="3">
-        <v>8023631111</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="3" customFormat="1" ht="98">
       <c r="A24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="3">
+        <v>8023631111</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="3" customFormat="1" ht="98">
+      <c r="A25" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B25" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D25" s="3">
         <v>8023631112</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E25" s="3" t="s">
         <v>229</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" s="3" customFormat="1" ht="42">
-      <c r="A25" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D25" s="7">
-        <v>24014</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A26" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="7">
+        <v>24014</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="3" customFormat="1" ht="42">
+      <c r="A27" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B27" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D27" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="E26" s="15" t="s">
+      <c r="E27" s="15" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="3" customFormat="1" ht="56">
-      <c r="A27" s="16" t="s">
+    <row r="28" spans="1:5" s="3" customFormat="1" ht="56">
+      <c r="A28" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B28" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D28" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="E27" s="15" t="s">
+      <c r="E28" s="15" t="s">
         <v>232</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" s="3" customFormat="1" ht="42">
-      <c r="A28" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A29" s="3" t="s">
-        <v>156</v>
+        <v>19</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>164</v>
+        <v>19</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>130</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A30" s="3" t="s">
-        <v>20</v>
+        <v>156</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D30" s="3">
-        <v>135</v>
+        <v>164</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A31" s="3" t="s">
-        <v>116</v>
+        <v>20</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>165</v>
+        <v>20</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D31" s="3">
+        <v>135</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A32" s="3" t="s">
-        <v>153</v>
+        <v>116</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>131</v>
+        <v>165</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A33" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>131</v>
       </c>
       <c r="E33" s="15" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="3" customFormat="1" ht="42">
+      <c r="A34" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E34" s="15" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="10" t="s">
+    <row r="35" spans="1:5">
+      <c r="A35" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-    </row>
-    <row r="35" spans="1:5" s="3" customFormat="1" ht="42">
-      <c r="A35" s="3" t="s">
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+    </row>
+    <row r="36" spans="1:5" s="3" customFormat="1" ht="42">
+      <c r="A36" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B36" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C36" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D36" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E36" s="3" t="s">
         <v>239</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" s="3" customFormat="1" ht="56">
-      <c r="A36" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="3" customFormat="1" ht="56">
       <c r="A37" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="3" customFormat="1" ht="56">
+      <c r="A38" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B38" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C38" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D38" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E38" s="3" t="s">
         <v>241</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" s="3" customFormat="1" ht="42">
-      <c r="A38" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D38" s="3">
-        <v>2015</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A39" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>134</v>
+        <v>23</v>
+      </c>
+      <c r="D39" s="3">
+        <v>2015</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A40" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A41" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" s="3" customFormat="1" ht="42">
+      <c r="A42" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B42" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C42" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D42" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="E42" s="3" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="3" customFormat="1" ht="42">
-      <c r="A42" s="16" t="s">
+    <row r="43" spans="1:5" s="3" customFormat="1" ht="42">
+      <c r="A43" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B43" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C43" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="D42" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" s="3" customFormat="1" ht="56">
-      <c r="A43" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="D43" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E43" s="3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" s="3" customFormat="1" ht="56">
+      <c r="A44" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D44" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E44" s="3" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="10" t="s">
+    <row r="45" spans="1:5">
+      <c r="A45" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-    </row>
-    <row r="45" spans="1:5" s="3" customFormat="1" ht="68" customHeight="1">
-      <c r="A45" s="14" t="s">
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+    </row>
+    <row r="46" spans="1:5" s="3" customFormat="1" ht="68" customHeight="1">
+      <c r="A46" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B46" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C46" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D46" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="E46" s="2" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="3" customFormat="1" ht="42">
-      <c r="A46" s="3" t="s">
+    <row r="47" spans="1:5" s="3" customFormat="1" ht="42">
+      <c r="A47" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B47" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C47" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D46" s="7" t="s">
+      <c r="D47" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="E46" s="15" t="s">
+      <c r="E47" s="15" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="3" customFormat="1" ht="56">
-      <c r="A47" s="3" t="s">
+    <row r="48" spans="1:5" s="3" customFormat="1" ht="56">
+      <c r="A48" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B48" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C48" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E47" s="15" t="s">
+      <c r="E48" s="15" t="s">
         <v>250</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" s="3" customFormat="1" ht="56">
-      <c r="A48" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="E48" s="15" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="49" spans="1:5" s="3" customFormat="1" ht="56">
       <c r="A49" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E49" s="15" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" s="3" customFormat="1" ht="56">
+      <c r="A50" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B50" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C50" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D50" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="E49" s="15" t="s">
+      <c r="E50" s="15" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="50" spans="1:5" s="3" customFormat="1" ht="42">
-      <c r="A50" s="3" t="s">
+    <row r="51" spans="1:5" s="3" customFormat="1" ht="42">
+      <c r="A51" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B51" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C51" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D51" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="E50" s="15" t="s">
+      <c r="E51" s="15" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="3" customFormat="1" ht="28">
-      <c r="A51" s="3" t="s">
+    <row r="52" spans="1:5" s="3" customFormat="1" ht="28">
+      <c r="A52" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B52" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C52" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D51" s="3">
+      <c r="D52" s="3">
         <v>0.2</v>
       </c>
-      <c r="E51" s="15" t="s">
+      <c r="E52" s="15" t="s">
         <v>254</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" s="3" customFormat="1" ht="56">
-      <c r="A52" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D52" s="3">
-        <v>30</v>
-      </c>
-      <c r="E52" s="15" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="53" spans="1:5" s="3" customFormat="1" ht="56">
       <c r="A53" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D53" s="3">
+        <v>30</v>
+      </c>
+      <c r="E53" s="15" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" s="3" customFormat="1" ht="56">
+      <c r="A54" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B54" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="D54" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E53" s="15" t="s">
+      <c r="E54" s="15" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="3" customFormat="1" ht="42">
-      <c r="A54" s="3" t="s">
+    <row r="55" spans="1:5" s="3" customFormat="1" ht="42">
+      <c r="A55" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B55" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C55" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D54" s="3">
+      <c r="D55" s="3">
         <v>40</v>
       </c>
-      <c r="E54" s="15" t="s">
+      <c r="E55" s="15" t="s">
         <v>257</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" s="3" customFormat="1" ht="56">
-      <c r="A55" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="E55" s="15" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="56" spans="1:5" s="3" customFormat="1" ht="56">
       <c r="A56" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="E56" s="15" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" s="3" customFormat="1" ht="56">
+      <c r="A57" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B57" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C57" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="D56" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E56" s="15" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" s="3" customFormat="1" ht="56">
-      <c r="A57" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="D57" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E57" s="15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="58" spans="1:5" s="3" customFormat="1" ht="56">
       <c r="A58" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D58" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E58" s="15" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" s="3" customFormat="1" ht="56">
+      <c r="A59" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D59" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E59" s="15" t="s">
         <v>261</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="56">
-      <c r="A59" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D59" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E59" s="15" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="56">
       <c r="A60" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D60" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E60" s="15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="56">
       <c r="A61" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D61" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E61" s="15" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="56">
       <c r="A62" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D62" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E62" s="15" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="56">
+      <c r="A63" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B63" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D62" s="2" t="s">
+      <c r="D63" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="E62" s="15" t="s">
+      <c r="E63" s="15" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
-      <c r="A63" s="10" t="s">
+    <row r="64" spans="1:5">
+      <c r="A64" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
-      <c r="E63" s="5"/>
-    </row>
-    <row r="64" spans="1:5" s="3" customFormat="1" ht="28">
-      <c r="A64" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>266</v>
-      </c>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
     </row>
     <row r="65" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A65" s="6" t="s">
-        <v>112</v>
+        <v>159</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>75</v>
+        <v>184</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="66" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A66" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" s="3" customFormat="1" ht="28">
+      <c r="A67" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B67" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="C67" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D66" s="3" t="s">
+      <c r="D67" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="E66" s="3" t="s">
+      <c r="E67" s="3" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="67" spans="1:5" s="3" customFormat="1" ht="28">
-      <c r="A67" s="3" t="s">
+    <row r="68" spans="1:5" s="3" customFormat="1" ht="28">
+      <c r="A68" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="B68" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="C68" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D67" s="3" t="s">
+      <c r="D68" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="E67" s="3" t="s">
+      <c r="E68" s="3" t="s">
         <v>269</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" s="3" customFormat="1" ht="28">
-      <c r="A68" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D68" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="69" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A69" s="6" t="s">
-        <v>114</v>
+        <v>160</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>78</v>
+        <v>185</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D69" s="3">
-        <v>2</v>
+        <v>55</v>
+      </c>
+      <c r="D69" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="70" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A70" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D70" s="8">
-        <v>47</v>
-      </c>
-      <c r="E70" s="8" t="s">
-        <v>272</v>
+        <v>44</v>
+      </c>
+      <c r="D70" s="3">
+        <v>2</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="71" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A71" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D71" s="8">
+        <v>47</v>
+      </c>
+      <c r="E71" s="8" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" s="3" customFormat="1" ht="28">
+      <c r="A72" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B72" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C71" s="3" t="s">
+      <c r="C72" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D71" s="8">
+      <c r="D72" s="8">
         <v>1197</v>
       </c>
-      <c r="E71" s="8" t="s">
+      <c r="E72" s="8" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
-      <c r="A72" s="10" t="s">
+    <row r="73" spans="1:5">
+      <c r="A73" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B72" s="5"/>
-      <c r="C72" s="5"/>
-      <c r="D72" s="5"/>
-      <c r="E72" s="5"/>
-    </row>
-    <row r="73" spans="1:5" s="3" customFormat="1" ht="56">
-      <c r="A73" s="3" t="s">
+      <c r="B73" s="5"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
+      <c r="E73" s="5"/>
+    </row>
+    <row r="74" spans="1:5" s="3" customFormat="1" ht="56">
+      <c r="A74" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B74" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C73" s="3" t="s">
+      <c r="C74" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D73" s="3" t="s">
+      <c r="D74" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="E73" s="3" t="s">
+      <c r="E74" s="3" t="s">
         <v>281</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" s="3" customFormat="1" ht="28">
-      <c r="A74" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="E74" s="3" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="75" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A75" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" s="3" customFormat="1" ht="28">
+      <c r="A76" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B76" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C75" s="3" t="s">
+      <c r="C76" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D75" s="3">
+      <c r="D76" s="3">
         <v>12345</v>
       </c>
-      <c r="E75" s="3" t="s">
+      <c r="E76" s="3" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="76" spans="1:5" s="3" customFormat="1" ht="42">
-      <c r="A76" s="3" t="s">
+    <row r="77" spans="1:5" s="3" customFormat="1" ht="42">
+      <c r="A77" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B77" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="C76" s="3" t="s">
+      <c r="C77" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D76" s="3" t="s">
+      <c r="D77" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="E76" s="3" t="s">
+      <c r="E77" s="3" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="77" spans="1:5" s="3" customFormat="1" ht="28">
-      <c r="A77" s="3" t="s">
+    <row r="78" spans="1:5" s="3" customFormat="1" ht="28">
+      <c r="A78" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B78" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C77" s="3" t="s">
+      <c r="C78" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D77" s="3" t="s">
+      <c r="D78" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="E77" s="3" t="s">
+      <c r="E78" s="3" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
-      <c r="A78" s="10" t="s">
+    <row r="79" spans="1:5">
+      <c r="A79" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="B78" s="5"/>
-      <c r="C78" s="5"/>
-      <c r="D78" s="5"/>
-      <c r="E78" s="5"/>
-    </row>
-    <row r="79" spans="1:5" ht="42">
-      <c r="A79" s="3" t="s">
+      <c r="B79" s="5"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="5"/>
+    </row>
+    <row r="80" spans="1:5" ht="42">
+      <c r="A80" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B80" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C79" s="3" t="s">
+      <c r="C80" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D79" s="3" t="s">
+      <c r="D80" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="E79" s="3" t="s">
+      <c r="E80" s="3" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="42">
-      <c r="A80" s="14" t="s">
+    <row r="81" spans="1:5" ht="42">
+      <c r="A81" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B81" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="C81" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D80" s="2" t="s">
+      <c r="D81" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="E80" s="3" t="s">
+      <c r="E81" s="3" t="s">
         <v>276</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" ht="56">
-      <c r="A81" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="E81" s="3" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="56">
       <c r="A82" s="3" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="56">
       <c r="A83" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="56">
       <c r="A84" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="56">
+      <c r="A85" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="B85" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C84" s="3" t="s">
+      <c r="C85" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D84" s="3" t="s">
+      <c r="D85" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="E84" s="3" t="s">
+      <c r="E85" s="3" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="85" spans="1:5">
-      <c r="A85" s="10" t="s">
+    <row r="86" spans="1:5">
+      <c r="A86" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="B85" s="5"/>
-      <c r="C85" s="5"/>
-      <c r="D85" s="5"/>
-      <c r="E85" s="5"/>
-    </row>
-    <row r="86" spans="1:5" ht="56">
-      <c r="A86" s="12" t="s">
+      <c r="B86" s="5"/>
+      <c r="C86" s="5"/>
+      <c r="D86" s="5"/>
+      <c r="E86" s="5"/>
+    </row>
+    <row r="87" spans="1:5" ht="56">
+      <c r="A87" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B87" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C86" s="2" t="s">
+      <c r="C87" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D86" s="2" t="b">
+      <c r="D87" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="E86" s="15" t="s">
+      <c r="E87" s="15" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="119" customHeight="1">
-      <c r="A87" s="17" t="s">
+    <row r="88" spans="1:5" ht="119" customHeight="1">
+      <c r="A88" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="B87" s="18"/>
-      <c r="C87" s="18"/>
-      <c r="D87" s="18"/>
+      <c r="B88" s="18"/>
+      <c r="C88" s="18"/>
+      <c r="D88" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A87:D87"/>
+    <mergeCell ref="A88:D88"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>